<commit_message>
#49 added updated report
</commit_message>
<xml_diff>
--- a/reports/20231220-provisioned-single-DB/PerfTestAnalysis.xlsx
+++ b/reports/20231220-provisioned-single-DB/PerfTestAnalysis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/roncewind/senzing.git/aws-cloudformation-performance-testing/reports/20231220-provisioned-single-DB/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E420CF70-02C0-7C48-A23E-1779536F6E62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44242DB0-EE70-B34D-9C60-36CD79B1BF82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="440" yWindow="500" windowWidth="35400" windowHeight="19700" xr2:uid="{83921CF5-0249-C341-948E-004987EBA171}"/>
   </bookViews>
@@ -549,6 +549,11 @@
                 </a:outerShdw>
               </a:effectLst>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000011-6A24-3B45-A3EB-EFCB3F902000}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="11"/>
@@ -594,6 +599,11 @@
                 </a:outerShdw>
               </a:effectLst>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000015-6A24-3B45-A3EB-EFCB3F902000}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="13"/>
@@ -616,6 +626,11 @@
                 </a:outerShdw>
               </a:effectLst>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000017-6A24-3B45-A3EB-EFCB3F902000}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dLbls>
             <c:spPr>
@@ -1379,6 +1394,11 @@
                 </a:outerShdw>
               </a:effectLst>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000F-C9F3-F845-8FA1-17F68A13D60F}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="11"/>
@@ -1424,6 +1444,11 @@
                 </a:outerShdw>
               </a:effectLst>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000013-C9F3-F845-8FA1-17F68A13D60F}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="13"/>
@@ -1446,6 +1471,11 @@
                 </a:outerShdw>
               </a:effectLst>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000015-C9F3-F845-8FA1-17F68A13D60F}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dLbls>
             <c:spPr>
@@ -2093,6 +2123,11 @@
                 </a:outerShdw>
               </a:effectLst>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000005-B47B-414F-9871-676D90298B07}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="8"/>
@@ -2163,6 +2198,11 @@
                 </a:outerShdw>
               </a:effectLst>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000B-B47B-414F-9871-676D90298B07}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="11"/>
@@ -2208,6 +2248,11 @@
                 </a:outerShdw>
               </a:effectLst>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000F-B47B-414F-9871-676D90298B07}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="13"/>
@@ -2230,6 +2275,11 @@
                 </a:outerShdw>
               </a:effectLst>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000011-B47B-414F-9871-676D90298B07}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dLbls>
             <c:spPr>
@@ -2870,6 +2920,11 @@
                 </a:outerShdw>
               </a:effectLst>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000005-9D14-9844-9646-9212059B3DEC}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="8"/>
@@ -2940,6 +2995,11 @@
                 </a:outerShdw>
               </a:effectLst>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000B-9D14-9844-9646-9212059B3DEC}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="11"/>
@@ -2985,6 +3045,11 @@
                 </a:outerShdw>
               </a:effectLst>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000F-9D14-9844-9646-9212059B3DEC}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="13"/>
@@ -3007,6 +3072,11 @@
                 </a:outerShdw>
               </a:effectLst>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000011-9D14-9844-9646-9212059B3DEC}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dLbls>
             <c:spPr>
@@ -3640,6 +3710,11 @@
                 </a:outerShdw>
               </a:effectLst>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000005-9E40-2A45-BCA6-D483BB8C3730}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="8"/>
@@ -3710,6 +3785,11 @@
                 </a:outerShdw>
               </a:effectLst>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000B-9E40-2A45-BCA6-D483BB8C3730}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="11"/>
@@ -3755,6 +3835,11 @@
                 </a:outerShdw>
               </a:effectLst>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000F-9E40-2A45-BCA6-D483BB8C3730}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="13"/>
@@ -3777,6 +3862,11 @@
                 </a:outerShdw>
               </a:effectLst>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000011-9E40-2A45-BCA6-D483BB8C3730}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dLbls>
             <c:spPr>
@@ -4381,6 +4471,31 @@
             </c:extLst>
           </c:dPt>
           <c:dPt>
+            <c:idx val="4"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="63000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000A-BFA2-A54D-B41F-6ED46289B5C7}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
             <c:idx val="6"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
@@ -4399,6 +4514,36 @@
                 </a:outerShdw>
               </a:effectLst>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000005-BFA2-A54D-B41F-6ED46289B5C7}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="7"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="63000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000B-BFA2-A54D-B41F-6ED46289B5C7}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="12"/>
@@ -4419,6 +4564,11 @@
                 </a:outerShdw>
               </a:effectLst>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000007-BFA2-A54D-B41F-6ED46289B5C7}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="13"/>
@@ -4441,6 +4591,11 @@
                 </a:outerShdw>
               </a:effectLst>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000009-BFA2-A54D-B41F-6ED46289B5C7}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dLbls>
             <c:spPr>
@@ -8648,8 +8803,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22BE6118-A1AB-0244-8A25-CA7A07813C69}">
   <dimension ref="B4:M251"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C250" sqref="C250"/>
+    <sheetView tabSelected="1" topLeftCell="A189" workbookViewId="0">
+      <selection activeCell="D263" sqref="D263"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>